<commit_message>
TC 03 modified. TC 01 and 04 in one Scenario Outline
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Brian\Automatizacion\CrowdarChallenge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Brian\Automatizacion\Selenium with Java\CrowdarChallenge\LoginChallenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="19560" windowHeight="8235" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="936" yWindow="0" windowWidth="22104" windowHeight="9780" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General_1" sheetId="2" state="hidden" r:id="rId1"/>
@@ -219,9 +219,6 @@
     <t>Successful login for valid user pressing Enter key</t>
   </si>
   <si>
-    <t>Successful login for invalid user</t>
-  </si>
-  <si>
     <t>Successful login due to slow loading</t>
   </si>
   <si>
@@ -373,9 +370,6 @@
     <t>The ecommerce landing page is displayed(header and footer page). Six products are displayed in the middle.</t>
   </si>
   <si>
-    <t>The ecommerce landing page is displayed(header and footer page). Six identical images of products are displayed in the middle.</t>
-  </si>
-  <si>
     <t>The ecommerce landing page is displayed in Chrome and Firefox browser.</t>
   </si>
   <si>
@@ -395,6 +389,12 @@
   </si>
   <si>
     <t>Click on Login button</t>
+  </si>
+  <si>
+    <t>Failed login for invalid user</t>
+  </si>
+  <si>
+    <t>The ecommerce landing page is displayed(header and footer page) and popup is also displayed for update personal information.</t>
   </si>
 </sst>
 </file>
@@ -686,7 +686,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -844,9 +844,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1220,22 +1217,22 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="4" width="24.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" customWidth="1"/>
+    <col min="3" max="4" width="24.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="7" max="8" width="16.109375" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" customWidth="1"/>
+    <col min="10" max="10" width="16.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" customWidth="1"/>
     <col min="12" max="12" width="11" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" customWidth="1"/>
-    <col min="19" max="20" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="62.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" customWidth="1"/>
+    <col min="19" max="20" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="62.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1300,7 +1297,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="18" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" s="18" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -1363,7 +1360,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>2</v>
       </c>
@@ -1429,7 +1426,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>3</v>
       </c>
@@ -1491,7 +1488,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>4</v>
       </c>
@@ -1552,7 +1549,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="29">
         <v>5</v>
       </c>
@@ -1611,7 +1608,7 @@
       </c>
       <c r="U7" s="34"/>
     </row>
-    <row r="8" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>6</v>
       </c>
@@ -1672,7 +1669,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="26">
         <v>7</v>
       </c>
@@ -1742,22 +1739,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="19"/>
-    <col min="2" max="2" width="46.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" customWidth="1"/>
-    <col min="4" max="4" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="19"/>
+    <col min="2" max="2" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.88671875" customWidth="1"/>
+    <col min="4" max="4" width="37.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="50" t="s">
         <v>54</v>
       </c>
@@ -1775,7 +1772,7 @@
       </c>
       <c r="F1" s="53"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="54" t="s">
         <v>56</v>
       </c>
@@ -1783,321 +1780,313 @@
         <v>57</v>
       </c>
       <c r="C2" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="49" t="s">
         <v>71</v>
-      </c>
-      <c r="D2" s="49" t="s">
-        <v>72</v>
       </c>
       <c r="E2" s="49" t="s">
         <v>58</v>
       </c>
       <c r="F2" s="53"/>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="60">
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="59">
         <v>1</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="68" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3" s="69" t="s">
+      <c r="C3" s="67" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="68" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="69" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="55"/>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="60">
+        <v>2</v>
+      </c>
+      <c r="B4" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="67" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="70" t="s">
-        <v>95</v>
-      </c>
-      <c r="F3" s="55"/>
-    </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="61">
-        <v>2</v>
-      </c>
-      <c r="B4" s="65" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="68" t="s">
-        <v>81</v>
-      </c>
-      <c r="D4" s="69" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" s="70" t="s">
-        <v>95</v>
+      <c r="E4" s="69" t="s">
+        <v>94</v>
       </c>
       <c r="F4" s="55"/>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="62">
-        <v>3</v>
-      </c>
-      <c r="B5" s="66" t="s">
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="60">
+        <v>4</v>
+      </c>
+      <c r="B5" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="68" t="s">
+      <c r="C5" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="D5" s="69" t="s">
+      <c r="D5" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="70" t="s">
-        <v>96</v>
+      <c r="E5" s="69" t="s">
+        <v>94</v>
       </c>
       <c r="F5" s="55"/>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="61">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="68" t="s">
+      <c r="C6" s="67" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="68" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="69" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="55"/>
+    </row>
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="62">
+        <v>6</v>
+      </c>
+      <c r="B7" s="65" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="D6" s="69" t="s">
-        <v>76</v>
-      </c>
-      <c r="E6" s="70" t="s">
-        <v>95</v>
-      </c>
-      <c r="F6" s="55"/>
-    </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="62">
-        <v>5</v>
-      </c>
-      <c r="B7" s="67" t="s">
+      <c r="D7" s="70" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="69" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" s="55"/>
+    </row>
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="59">
+        <v>7</v>
+      </c>
+      <c r="B8" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="68" t="s">
-        <v>93</v>
-      </c>
-      <c r="D7" s="69" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" s="70" t="s">
-        <v>97</v>
-      </c>
-      <c r="F7" s="55"/>
-    </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="63">
-        <v>6</v>
-      </c>
-      <c r="B8" s="66" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="68" t="s">
+      <c r="C8" s="67" t="s">
         <v>84</v>
       </c>
       <c r="D8" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="70" t="s">
+      <c r="E8" s="69" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" s="55"/>
+    </row>
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="62">
+        <v>8</v>
+      </c>
+      <c r="B9" s="65" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="67" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="68" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="69" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" s="55"/>
+    </row>
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="61">
+        <v>9</v>
+      </c>
+      <c r="B10" s="65" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="67" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="68" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="69" t="s">
         <v>98</v>
       </c>
-      <c r="F8" s="55"/>
-    </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="60">
-        <v>7</v>
-      </c>
-      <c r="B9" s="66" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="68" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" s="72" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" s="70" t="s">
+      <c r="F10" s="55"/>
+    </row>
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="62">
+        <v>10</v>
+      </c>
+      <c r="B11" s="65" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="67" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="69" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="55"/>
+    </row>
+    <row r="12" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="61">
+        <v>11</v>
+      </c>
+      <c r="B12" s="65" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="72" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="68" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" s="69" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" s="55"/>
+    </row>
+    <row r="13" spans="1:6" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="62">
+        <v>12</v>
+      </c>
+      <c r="B13" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="68" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" s="69" t="s">
         <v>99</v>
       </c>
-      <c r="F9" s="55"/>
-    </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="63">
-        <v>8</v>
-      </c>
-      <c r="B10" s="66" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="68" t="s">
+      <c r="F13" s="55"/>
+    </row>
+    <row r="14" spans="1:6" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="61">
+        <v>13</v>
+      </c>
+      <c r="B14" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="68" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="69" t="s">
+        <v>100</v>
+      </c>
+      <c r="F14" s="55"/>
+    </row>
+    <row r="15" spans="1:6" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="61">
+        <v>3</v>
+      </c>
+      <c r="B15" s="65" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="69" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="70" t="s">
-        <v>95</v>
-      </c>
-      <c r="F10" s="55"/>
-    </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="62">
-        <v>9</v>
-      </c>
-      <c r="B11" s="66" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="68" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="69" t="s">
-        <v>90</v>
-      </c>
-      <c r="E11" s="70" t="s">
-        <v>100</v>
-      </c>
-      <c r="F11" s="55"/>
-    </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="63">
-        <v>10</v>
-      </c>
-      <c r="B12" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="68" t="s">
-        <v>87</v>
-      </c>
-      <c r="D12" s="69" t="s">
-        <v>91</v>
-      </c>
-      <c r="E12" s="70" t="s">
-        <v>100</v>
-      </c>
-      <c r="F12" s="55"/>
-    </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="62">
-        <v>11</v>
-      </c>
-      <c r="B13" s="66" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" s="73" t="s">
-        <v>88</v>
-      </c>
-      <c r="D13" s="69" t="s">
+      <c r="D15" s="68" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="69" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="70" t="s">
-        <v>98</v>
-      </c>
-      <c r="F13" s="55"/>
-    </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="63">
-        <v>12</v>
-      </c>
-      <c r="B14" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" s="68" t="s">
-        <v>89</v>
-      </c>
-      <c r="D14" s="69" t="s">
-        <v>92</v>
-      </c>
-      <c r="E14" s="70" t="s">
-        <v>101</v>
-      </c>
-      <c r="F14" s="55"/>
-    </row>
-    <row r="15" spans="1:6" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="62">
-        <v>13</v>
-      </c>
-      <c r="B15" s="66" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="68" t="s">
-        <v>94</v>
-      </c>
-      <c r="D15" s="69" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" s="70" t="s">
-        <v>102</v>
-      </c>
       <c r="F15" s="55"/>
     </row>
-    <row r="16" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="56"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-    </row>
-    <row r="17" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="57"/>
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="58"/>
-    </row>
-    <row r="18" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="57"/>
-      <c r="B18" s="58"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="58"/>
-    </row>
-    <row r="19" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="57"/>
-      <c r="B19" s="58"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="58"/>
-    </row>
-    <row r="20" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="57"/>
-      <c r="B20" s="58"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="58"/>
-    </row>
-    <row r="21" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="57"/>
-      <c r="B21" s="58"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="58"/>
-    </row>
-    <row r="22" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="59"/>
-    </row>
-    <row r="23" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="59"/>
-    </row>
-    <row r="24" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="59"/>
-    </row>
-    <row r="25" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="59"/>
-    </row>
-    <row r="26" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="59"/>
-    </row>
-    <row r="27" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="59"/>
-    </row>
-    <row r="28" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="59"/>
-    </row>
-    <row r="29" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="59"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+    </row>
+    <row r="17" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="56"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+    </row>
+    <row r="18" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="56"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+    </row>
+    <row r="19" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="56"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+    </row>
+    <row r="20" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="56"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+    </row>
+    <row r="21" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="58"/>
+    </row>
+    <row r="22" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="58"/>
+    </row>
+    <row r="23" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="58"/>
+    </row>
+    <row r="24" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="58"/>
+    </row>
+    <row r="25" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="58"/>
+    </row>
+    <row r="26" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="58"/>
+    </row>
+    <row r="27" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="58"/>
+    </row>
+    <row r="28" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="58"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>